<commit_message>
Adição de validação de dados no Backlog
</commit_message>
<xml_diff>
--- a/Documentacao/Sprint 2/Backlog/HFSystem_Backlog.xlsx
+++ b/Documentacao/Sprint 2/Backlog/HFSystem_Backlog.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/945fbc0a8965b131/Desktop/HFSYSTEM/HFSystem/Documentacao/Sprint 2/Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\OneDrive\Pessoal\1 - Documentos\2 - Acessos\Desktop\Projetos\Projetos em grupo\HFSystem\Documentacao\Sprint 2\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{465695A6-03A4-4944-9DBA-1E1D54D4999F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41D4B896-75BE-43EE-A65E-76F1BBC48194}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C39593-2FE8-4513-81B6-DDD55B56D074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFSystem" sheetId="1" r:id="rId1"/>
+    <sheet name="Banco de dados" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HFSystem!$B$3:$J$46</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="106">
   <si>
     <t>BACKLOG</t>
   </si>
@@ -179,12 +180,6 @@
     <t>VALIDAÇÃO DE DIAGRAMA DE SOLUÇÃO (EXPLICAÇÃO PENDENTE)</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
     <t>DESEJÁVEL</t>
   </si>
   <si>
@@ -329,9 +324,6 @@
     <t>Vinicius</t>
   </si>
   <si>
-    <t>Feito</t>
-  </si>
-  <si>
     <t>PREVISTO</t>
   </si>
   <si>
@@ -345,13 +337,34 @@
   </si>
   <si>
     <t>STATUS</t>
+  </si>
+  <si>
+    <t>Classificação</t>
+  </si>
+  <si>
+    <t>DASHBOARD - BURNDOWN</t>
+  </si>
+  <si>
+    <t>A realizar</t>
+  </si>
+  <si>
+    <t>Realizando</t>
+  </si>
+  <si>
+    <t>Realizado</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,12 +412,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial Nova Light"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -438,7 +445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -498,11 +505,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0E617C"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0E617C"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0E617C"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0E617C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0E617C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0E617C"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0E617C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0E617C"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0E617C"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0E617C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0E617C"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0E617C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0E617C"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF0E617C"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0E617C"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -552,9 +645,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -564,19 +654,99 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0E617C"/>
       <color rgb="FF0078A6"/>
-      <color rgb="FF0E617C"/>
       <color rgb="FF5CE1E6"/>
       <color rgb="FF5DE0E6"/>
     </mruColors>
@@ -684,7 +854,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>HFSystem!$L$4:$L$8</c:f>
+              <c:f>HFSystem!$R$4:$R$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -707,7 +877,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>HFSystem!$M$4:$M$8</c:f>
+              <c:f>HFSystem!$S$4:$S$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -921,7 +1091,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>HFSystem!$L$4:$L$8</c:f>
+              <c:f>HFSystem!$R$4:$R$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -944,7 +1114,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>HFSystem!$N$4:$N$8</c:f>
+              <c:f>HFSystem!$T$4:$T$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1735,16 +1905,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>616085</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>6484</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>8106</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>40532</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>202660</xdr:rowOff>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2037,53 +2207,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:S46"/>
+  <dimension ref="B1:U46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="78.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="9"/>
+    <col min="1" max="1" width="1.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="86.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" style="9" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" style="9" customWidth="1"/>
     <col min="14" max="14" width="15" style="9" customWidth="1"/>
     <col min="15" max="15" width="14.85546875" style="9" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="9"/>
+    <col min="16" max="16" width="9.140625" style="9"/>
+    <col min="17" max="17" width="2.140625" style="9" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+    <row r="1" spans="2:21" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-    </row>
-    <row r="3" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="L2" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="32"/>
+      <c r="R2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+    </row>
+    <row r="3" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2094,47 +2277,52 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K3" s="10"/>
-      <c r="L3" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="L3" s="23"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="24"/>
+      <c r="R3" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="T3" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F4" s="6">
         <f>IF(E4="PP",3,IF(E4="P",5,IF(E4="M",8,IF(E4="G",13,21))))</f>
@@ -2144,44 +2332,48 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K4" s="10"/>
-      <c r="L4" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="M4" s="14">
-        <f>M5+M6+M7</f>
+      <c r="L4" s="23"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="24"/>
+      <c r="R4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="S4" s="14">
+        <f>S5+S6+S7</f>
         <v>449</v>
       </c>
-      <c r="N4" s="14">
-        <f>SUM(N5:N7)</f>
+      <c r="T4" s="14">
+        <f>SUM(T5:T7)</f>
         <v>449</v>
       </c>
-      <c r="O4" s="14">
-        <f>SUM(O5:O8)</f>
+      <c r="U4" s="14">
+        <f>SUM(U5:U8)</f>
         <v>184</v>
       </c>
-      <c r="S4" s="16"/>
-    </row>
-    <row r="5" spans="2:19" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:21" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" ref="F5:F46" si="0">IF(E5="PP",3,IF(E5="P",5,IF(E5="M",8,IF(E5="G",13,21))))</f>
@@ -2191,32 +2383,37 @@
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="M5" s="14">
+        <v>103</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="24"/>
+      <c r="R5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="14">
         <f>149</f>
         <v>149</v>
       </c>
-      <c r="N5" s="15">
+      <c r="T5" s="15">
         <f>SUM(F4:F18)</f>
         <v>118</v>
       </c>
-      <c r="O5" s="14">
+      <c r="U5" s="14">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>6</v>
@@ -2225,7 +2422,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="0"/>
@@ -2235,32 +2432,37 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M6" s="14">
+        <v>103</v>
+      </c>
+      <c r="L6" s="25"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="26"/>
+      <c r="R6" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="S6" s="14">
         <f>150</f>
         <v>150</v>
       </c>
-      <c r="N6" s="15">
+      <c r="T6" s="15">
         <f>SUM(F19:F33)</f>
         <v>134</v>
       </c>
-      <c r="O6" s="14">
+      <c r="U6" s="14">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>7</v>
@@ -2269,7 +2471,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
@@ -2279,31 +2481,36 @@
         <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="23"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="24"/>
+      <c r="R7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7" s="14">
+      <c r="S7" s="14">
         <v>150</v>
       </c>
-      <c r="N7" s="15">
+      <c r="T7" s="15">
         <f>SUM(F34:F46)</f>
         <v>197</v>
       </c>
-      <c r="O7" s="14">
+      <c r="U7" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>8</v>
@@ -2312,7 +2519,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="0"/>
@@ -2322,30 +2529,35 @@
         <v>3</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" s="14">
+        <v>103</v>
+      </c>
+      <c r="L8" s="23"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="24"/>
+      <c r="R8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="S8" s="14">
         <v>0</v>
       </c>
-      <c r="N8" s="14">
+      <c r="T8" s="14">
         <v>0</v>
       </c>
-      <c r="O8" s="14">
+      <c r="U8" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -2354,7 +2566,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="0"/>
@@ -2364,19 +2576,24 @@
         <v>3</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="L9" s="23"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="24"/>
+    </row>
+    <row r="10" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>11</v>
@@ -2385,7 +2602,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="0"/>
@@ -2395,19 +2612,24 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="L10" s="23"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="24"/>
+    </row>
+    <row r="11" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>12</v>
@@ -2416,7 +2638,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
@@ -2426,26 +2648,31 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="L11" s="23"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="24"/>
+    </row>
+    <row r="12" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B12" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="0"/>
@@ -2455,26 +2682,31 @@
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="L12" s="23"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="24"/>
+    </row>
+    <row r="13" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" si="0"/>
@@ -2484,28 +2716,33 @@
         <v>3</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="2:19" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="L13" s="23"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="24"/>
+    </row>
+    <row r="14" spans="2:21" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" si="0"/>
@@ -2515,19 +2752,24 @@
         <v>1</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="L14" s="23"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="24"/>
+    </row>
+    <row r="15" spans="2:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>14</v>
@@ -2536,7 +2778,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" si="0"/>
@@ -2546,19 +2788,24 @@
         <v>1</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="L15" s="27"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="29"/>
+    </row>
+    <row r="16" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>15</v>
@@ -2567,7 +2814,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" s="6">
         <f t="shared" si="0"/>
@@ -2577,20 +2824,20 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K16" s="10"/>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B17" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>16</v>
@@ -2599,7 +2846,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F17" s="6">
         <f t="shared" si="0"/>
@@ -2609,19 +2856,19 @@
         <v>3</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>17</v>
@@ -2630,7 +2877,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F18" s="6">
         <f t="shared" si="0"/>
@@ -2640,17 +2887,17 @@
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="11" t="s">
         <v>18</v>
       </c>
@@ -2661,7 +2908,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" s="6">
         <f t="shared" si="0"/>
@@ -2671,26 +2918,28 @@
         <v>2</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J19" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F20" s="6">
         <f t="shared" si="0"/>
@@ -2700,26 +2949,28 @@
         <v>3</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" si="0"/>
@@ -2729,15 +2980,17 @@
         <v>3</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J21" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
@@ -2748,7 +3001,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F22" s="6">
         <f t="shared" si="0"/>
@@ -2758,15 +3011,17 @@
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J22" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
@@ -2777,7 +3032,7 @@
         <v>10</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" s="6">
         <f t="shared" si="0"/>
@@ -2787,15 +3042,17 @@
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J23" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B24" s="11" t="s">
         <v>23</v>
       </c>
@@ -2806,7 +3063,7 @@
         <v>10</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F24" s="6">
         <f t="shared" si="0"/>
@@ -2816,15 +3073,17 @@
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J24" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B25" s="11" t="s">
         <v>24</v>
       </c>
@@ -2835,7 +3094,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F25" s="6">
         <f t="shared" si="0"/>
@@ -2845,17 +3104,19 @@
         <v>2</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B26" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>40</v>
@@ -2864,7 +3125,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="0"/>
@@ -2874,15 +3135,17 @@
         <v>2</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J26" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="s">
         <v>25</v>
       </c>
@@ -2893,7 +3156,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F27" s="6">
         <f t="shared" si="0"/>
@@ -2903,24 +3166,26 @@
         <v>2</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J27" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F28" s="6">
         <f t="shared" si="0"/>
@@ -2930,25 +3195,26 @@
         <v>2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J28" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K28" s="10"/>
-      <c r="L28" s="16"/>
-    </row>
-    <row r="29" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B29" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" si="0"/>
@@ -2958,15 +3224,17 @@
         <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B30" s="11" t="s">
         <v>26</v>
       </c>
@@ -2977,7 +3245,7 @@
         <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F30" s="6">
         <f t="shared" si="0"/>
@@ -2987,15 +3255,17 @@
         <v>2</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J30" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B31" s="11" t="s">
         <v>27</v>
       </c>
@@ -3006,7 +3276,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F31" s="6">
         <f t="shared" si="0"/>
@@ -3016,17 +3286,19 @@
         <v>2</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J31" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B32" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>44</v>
@@ -3035,7 +3307,7 @@
         <v>10</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F32" s="6">
         <f t="shared" si="0"/>
@@ -3045,12 +3317,14 @@
         <v>1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J32" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="K32" s="10"/>
     </row>
     <row r="33" spans="2:11" ht="18" x14ac:dyDescent="0.35">
@@ -3064,7 +3338,7 @@
         <v>10</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F33" s="6">
         <f t="shared" si="0"/>
@@ -3074,12 +3348,14 @@
         <v>3</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J33" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K33" s="10"/>
     </row>
     <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.35">
@@ -3087,13 +3363,13 @@
         <v>29</v>
       </c>
       <c r="C34" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E34" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F34" s="6">
         <f t="shared" si="0"/>
@@ -3103,12 +3379,14 @@
         <v>2</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J34" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="2:11" ht="18" x14ac:dyDescent="0.35">
@@ -3116,13 +3394,13 @@
         <v>30</v>
       </c>
       <c r="C35" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F35" s="6">
         <f t="shared" si="0"/>
@@ -3132,12 +3410,14 @@
         <v>3</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J35" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K35" s="10"/>
     </row>
     <row r="36" spans="2:11" ht="18" x14ac:dyDescent="0.35">
@@ -3145,13 +3425,13 @@
         <v>31</v>
       </c>
       <c r="C36" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E36" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F36" s="6">
         <f t="shared" si="0"/>
@@ -3161,12 +3441,14 @@
         <v>2</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J36" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K36" s="10"/>
     </row>
     <row r="37" spans="2:11" ht="18" x14ac:dyDescent="0.35">
@@ -3174,13 +3456,13 @@
         <v>32</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E37" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F37" s="6">
         <f t="shared" si="0"/>
@@ -3190,12 +3472,14 @@
         <v>1</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J37" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K37" s="10"/>
     </row>
     <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.35">
@@ -3203,13 +3487,13 @@
         <v>33</v>
       </c>
       <c r="C38" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E38" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F38" s="6">
         <f t="shared" si="0"/>
@@ -3219,24 +3503,26 @@
         <v>1</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J38" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K38" s="10"/>
     </row>
     <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B39" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F39" s="6">
         <f t="shared" si="0"/>
@@ -3246,24 +3532,26 @@
         <v>2</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J39" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K39" s="10"/>
     </row>
     <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B40" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F40" s="6">
         <f t="shared" si="0"/>
@@ -3273,24 +3561,26 @@
         <v>3</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J40" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K40" s="10"/>
     </row>
     <row r="41" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B41" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F41" s="6">
         <f t="shared" si="0"/>
@@ -3300,24 +3590,26 @@
         <v>2</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J41" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K41" s="10"/>
     </row>
     <row r="42" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B42" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F42" s="6">
         <f t="shared" si="0"/>
@@ -3327,24 +3619,26 @@
         <v>2</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J42" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K42" s="10"/>
     </row>
     <row r="43" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B43" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F43" s="6">
         <f t="shared" si="0"/>
@@ -3354,24 +3648,26 @@
         <v>1</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J43" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K43" s="10"/>
     </row>
     <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B44" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F44" s="6">
         <f t="shared" si="0"/>
@@ -3381,24 +3677,26 @@
         <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J44" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K44" s="10"/>
     </row>
     <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B45" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F45" s="6">
         <f t="shared" si="0"/>
@@ -3408,12 +3706,14 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J45" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K45" s="10"/>
     </row>
     <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.35">
@@ -3421,13 +3721,13 @@
         <v>34</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E46" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F46" s="6">
         <f t="shared" si="0"/>
@@ -3437,31 +3737,155 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J46" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K46" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:J46" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="L2:P2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E46" xr:uid="{367C11EB-FC9E-42D9-AD1B-E8D3575B0C70}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H46 J19:J46" xr:uid="{60436FE9-F290-49A5-AF78-C5478B063B7C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H46" xr:uid="{60436FE9-F290-49A5-AF78-C5478B063B7C}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{56A57BB8-5038-40B3-B0B8-425BF2D3D617}">
+            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$2,J4)))</xm:f>
+            <xm:f>'Banco de dados'!$B$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J4:J46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{DAC070DB-A49A-401D-A275-DDA2BD6A97CB}">
+            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$4,J4)))</xm:f>
+            <xm:f>'Banco de dados'!$B$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF00B050"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{7B148E7E-E100-47C8-948B-3C7AD8AB7191}">
+            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$3,J4)))</xm:f>
+            <xm:f>'Banco de dados'!$B$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J4:J46</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{92CE0B0A-37DF-4939-816D-81E895BC8B62}">
+          <x14:formula1>
+            <xm:f>'Banco de dados'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>J4:J46</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCB23AFF-6DEB-4467-B2E8-5C3C9F00F886}">
+          <x14:formula1>
+            <xm:f>'Banco de dados'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4:D46</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B0F8FD-0295-424D-BFA2-4D3F6325DB71}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adição da descrição dos entregaveis no backlog
</commit_message>
<xml_diff>
--- a/Documentacao/Sprint 2/Backlog/HFSystem_Backlog.xlsx
+++ b/Documentacao/Sprint 2/Backlog/HFSystem_Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\OneDrive\Pessoal\1 - Documentos\2 - Acessos\Desktop\Projetos\Projetos em grupo\HFSystem\Documentacao\Sprint 2\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\OneDrive\Pessoal\1 - Documentos\2 - Acessos\Desktop\Projetos\Projetos em grupo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C39593-2FE8-4513-81B6-DDD55B56D074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA3661A-3396-4253-90B9-06B1A9F4B951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFSystem" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="120">
   <si>
     <t>BACKLOG</t>
   </si>
@@ -357,7 +357,49 @@
     <t>Status</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>LOCAÇÃO DOS ELEMENTOS DO PROJETO EM UM REPOSITÓRIO NO GITHUB</t>
+  </si>
+  <si>
+    <t>CONFIGURAÇÃO DE TODOS OS ENTREGÁVEIS NO TRELLO</t>
+  </si>
+  <si>
+    <t>CRIAÇÃO DE PLANILHA DE RISCOS JUNTAMENTE COM GRÁFICO DE BURNDOWN</t>
+  </si>
+  <si>
+    <t>MODELAGEM DO BANCO DE DADOS</t>
+  </si>
+  <si>
+    <t>UTILIZAÇÃO DO SENSOR JUNTO COM A API</t>
+  </si>
+  <si>
+    <t>CRIAÇÃO DO BACKLOG</t>
+  </si>
+  <si>
+    <t>CRIAÇÃO DE UMA DASHBOARD ESTÁTICA</t>
+  </si>
+  <si>
+    <t>CRIAÇÃO E CONFIGURAÇÃO DE UMA DASHBOARD FUNCIONAL</t>
+  </si>
+  <si>
+    <t>CRIAÇÃO DE PÁGINA DE LOGIN E CADASTRO FUNCIONAL</t>
+  </si>
+  <si>
+    <t>A DEFINIR</t>
+  </si>
+  <si>
+    <t>CRIAÇÃO DE MODELAGEM DEFINITIVA DO PROJETO</t>
+  </si>
+  <si>
+    <t>CRIAÇÃO DE SITE INSTITUCIONAL EM HTML/CSS/JS FUNCIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A DEFINIR </t>
+  </si>
+  <si>
+    <t>SINCRONIZAÇÃO DOS DADOS CAPTADOS PELO SENSOR COM A API</t>
+  </si>
+  <si>
+    <t>INTEGRAÇÃO DO ARDUINO COM O BANCO DE DADOS</t>
   </si>
 </sst>
 </file>
@@ -595,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -645,24 +687,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,6 +708,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,14 +732,24 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -718,26 +767,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2209,64 +2238,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:U46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="86.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="123.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="86.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="17" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.140625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="9" customWidth="1"/>
     <col min="14" max="14" width="15" style="9" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" style="9" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="9"/>
-    <col min="17" max="17" width="2.140625" style="9" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" style="9" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="9"/>
+    <col min="17" max="17" width="2.109375" style="9" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="9"/>
+    <col min="20" max="20" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="17" t="s">
+    <row r="1" spans="2:21" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="32"/>
-      <c r="R2" s="20" t="s">
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="31"/>
+      <c r="R2" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-    </row>
-    <row r="3" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+    </row>
+    <row r="3" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2295,29 +2324,28 @@
         <v>98</v>
       </c>
       <c r="K3" s="10"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="24"/>
-      <c r="R3" s="33" t="s">
+      <c r="L3" s="17"/>
+      <c r="P3" s="18"/>
+      <c r="R3" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="S3" s="33" t="s">
+      <c r="S3" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="T3" s="33" t="s">
+      <c r="T3" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="U3" s="33" t="s">
+      <c r="U3" s="24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
@@ -2341,11 +2369,8 @@
         <v>103</v>
       </c>
       <c r="K4" s="10"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="24"/>
+      <c r="L4" s="17"/>
+      <c r="P4" s="18"/>
       <c r="R4" s="14" t="s">
         <v>84</v>
       </c>
@@ -2362,7 +2387,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="2:21" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:21" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
         <v>60</v>
       </c>
@@ -2391,11 +2416,11 @@
       <c r="J5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="24"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="18"/>
       <c r="R5" s="14" t="s">
         <v>55</v>
       </c>
@@ -2411,7 +2436,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B6" s="11" t="s">
         <v>58</v>
       </c>
@@ -2440,11 +2465,11 @@
       <c r="J6" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="25"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="26"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="20"/>
       <c r="R6" s="14" t="s">
         <v>56</v>
       </c>
@@ -2460,7 +2485,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B7" s="11" t="s">
         <v>61</v>
       </c>
@@ -2489,11 +2514,8 @@
       <c r="J7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="24"/>
+      <c r="L7" s="17"/>
+      <c r="P7" s="18"/>
       <c r="R7" s="14" t="s">
         <v>57</v>
       </c>
@@ -2508,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>67</v>
       </c>
@@ -2537,11 +2559,8 @@
       <c r="J8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="24"/>
+      <c r="L8" s="17"/>
+      <c r="P8" s="18"/>
       <c r="R8" s="14" t="s">
         <v>85</v>
       </c>
@@ -2555,7 +2574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B9" s="11" t="s">
         <v>83</v>
       </c>
@@ -2585,13 +2604,10 @@
         <v>103</v>
       </c>
       <c r="K9" s="10"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="24"/>
-    </row>
-    <row r="10" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="L9" s="17"/>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B10" s="11" t="s">
         <v>62</v>
       </c>
@@ -2621,13 +2637,10 @@
         <v>103</v>
       </c>
       <c r="K10" s="10"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="24"/>
-    </row>
-    <row r="11" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="L10" s="17"/>
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B11" s="11" t="s">
         <v>63</v>
       </c>
@@ -2657,17 +2670,16 @@
         <v>103</v>
       </c>
       <c r="K11" s="10"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="24"/>
-    </row>
-    <row r="12" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="L11" s="17"/>
+      <c r="P11" s="18"/>
+    </row>
+    <row r="12" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2691,17 +2703,16 @@
         <v>103</v>
       </c>
       <c r="K12" s="10"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="24"/>
-    </row>
-    <row r="13" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="L12" s="17"/>
+      <c r="P12" s="18"/>
+    </row>
+    <row r="13" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
@@ -2725,13 +2736,10 @@
         <v>103</v>
       </c>
       <c r="K13" s="10"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="24"/>
-    </row>
-    <row r="14" spans="2:21" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="L13" s="17"/>
+      <c r="P13" s="18"/>
+    </row>
+    <row r="14" spans="2:21" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
       <c r="B14" s="12" t="s">
         <v>66</v>
       </c>
@@ -2761,13 +2769,13 @@
         <v>103</v>
       </c>
       <c r="K14" s="10"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="24"/>
-    </row>
-    <row r="15" spans="2:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L14" s="17"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="18"/>
+    </row>
+    <row r="15" spans="2:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="11" t="s">
         <v>68</v>
       </c>
@@ -2797,13 +2805,13 @@
         <v>103</v>
       </c>
       <c r="K15" s="10"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="29"/>
-    </row>
-    <row r="16" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="L15" s="21"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="23"/>
+    </row>
+    <row r="16" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B16" s="11" t="s">
         <v>69</v>
       </c>
@@ -2835,7 +2843,7 @@
       <c r="K16" s="10"/>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B17" s="11" t="s">
         <v>70</v>
       </c>
@@ -2866,7 +2874,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B18" s="11" t="s">
         <v>71</v>
       </c>
@@ -2897,7 +2905,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B19" s="11" t="s">
         <v>18</v>
       </c>
@@ -2928,12 +2936,12 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
@@ -2959,12 +2967,12 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
@@ -2990,7 +2998,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
@@ -3021,7 +3029,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
@@ -3052,7 +3060,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B24" s="11" t="s">
         <v>23</v>
       </c>
@@ -3083,7 +3091,7 @@
       </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B25" s="11" t="s">
         <v>24</v>
       </c>
@@ -3114,7 +3122,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B26" s="11" t="s">
         <v>72</v>
       </c>
@@ -3145,7 +3153,7 @@
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B27" s="11" t="s">
         <v>25</v>
       </c>
@@ -3176,11 +3184,13 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B28" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>10</v>
       </c>
@@ -3205,11 +3215,13 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B29" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>10</v>
       </c>
@@ -3234,7 +3246,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B30" s="11" t="s">
         <v>26</v>
       </c>
@@ -3265,7 +3277,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B31" s="11" t="s">
         <v>27</v>
       </c>
@@ -3296,7 +3308,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B32" s="11" t="s">
         <v>75</v>
       </c>
@@ -3327,7 +3339,7 @@
       </c>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B33" s="11" t="s">
         <v>28</v>
       </c>
@@ -3358,12 +3370,12 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B34" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>46</v>
@@ -3389,12 +3401,12 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B35" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>46</v>
@@ -3420,12 +3432,12 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B36" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>105</v>
+      <c r="C36" s="32" t="s">
+        <v>118</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>46</v>
@@ -3451,12 +3463,12 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B37" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>46</v>
@@ -3482,12 +3494,12 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B38" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>46</v>
@@ -3513,11 +3525,13 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B39" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="11"/>
+      <c r="C39" s="11" t="s">
+        <v>115</v>
+      </c>
       <c r="D39" s="2" t="s">
         <v>46</v>
       </c>
@@ -3542,11 +3556,13 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B40" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="D40" s="2" t="s">
         <v>46</v>
       </c>
@@ -3571,11 +3587,13 @@
       </c>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B41" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="11"/>
+      <c r="C41" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="D41" s="2" t="s">
         <v>46</v>
       </c>
@@ -3600,11 +3618,13 @@
       </c>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B42" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="11"/>
+      <c r="C42" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="D42" s="2" t="s">
         <v>46</v>
       </c>
@@ -3629,11 +3649,13 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="11"/>
+      <c r="C43" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="D43" s="2" t="s">
         <v>46</v>
       </c>
@@ -3658,11 +3680,13 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B44" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C44" s="11" t="s">
+        <v>112</v>
+      </c>
       <c r="D44" s="2" t="s">
         <v>46</v>
       </c>
@@ -3687,11 +3711,13 @@
       </c>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B45" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="11"/>
+      <c r="C45" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="D45" s="2" t="s">
         <v>46</v>
       </c>
@@ -3716,12 +3742,12 @@
       </c>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.45">
       <c r="B46" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>46</v>
@@ -3770,23 +3796,20 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{56A57BB8-5038-40B3-B0B8-425BF2D3D617}">
-            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$2,J4)))</xm:f>
-            <xm:f>'Banco de dados'!$B$2</xm:f>
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{7B148E7E-E100-47C8-948B-3C7AD8AB7191}">
+            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$3,J4)))</xm:f>
+            <xm:f>'Banco de dados'!$B$3</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FFFF0000"/>
+                <color theme="7"/>
               </font>
               <fill>
                 <patternFill>
-                  <bgColor theme="5" tint="0.79998168889431442"/>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>J4:J46</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{DAC070DB-A49A-401D-A275-DDA2BD6A97CB}">
             <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$4,J4)))</xm:f>
             <xm:f>'Banco de dados'!$B$4</xm:f>
@@ -3801,16 +3824,16 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{7B148E7E-E100-47C8-948B-3C7AD8AB7191}">
-            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$3,J4)))</xm:f>
-            <xm:f>'Banco de dados'!$B$3</xm:f>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{56A57BB8-5038-40B3-B0B8-425BF2D3D617}">
+            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$2,J4)))</xm:f>
+            <xm:f>'Banco de dados'!$B$2</xm:f>
             <x14:dxf>
               <font>
-                <color theme="7"/>
+                <color rgb="FFFF0000"/>
               </font>
               <fill>
                 <patternFill>
-                  <bgColor theme="7" tint="0.79998168889431442"/>
+                  <bgColor theme="5" tint="0.79998168889431442"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -3847,13 +3870,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>99</v>
       </c>
@@ -3861,7 +3884,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3869,7 +3892,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3877,7 +3900,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
wallpaper fundo da vm
</commit_message>
<xml_diff>
--- a/Documentacao/Sprint 2/Backlog/HFSystem_Backlog.xlsx
+++ b/Documentacao/Sprint 2/Backlog/HFSystem_Backlog.xlsx
@@ -5,19 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\OneDrive\Pessoal\1 - Documentos\2 - Acessos\Desktop\Projetos\Projetos em grupo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\SPtech\HFSystem\Documentacao\Sprint 2\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA3661A-3396-4253-90B9-06B1A9F4B951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED625A1-3058-4C4D-9028-AA950374FD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5184" yWindow="348" windowWidth="17856" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFSystem" sheetId="1" r:id="rId1"/>
-    <sheet name="Banco de dados" sheetId="2" r:id="rId2"/>
+    <sheet name="HFSystem (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Banco de dados" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HFSystem!$B$3:$J$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'HFSystem (2)'!$B$3:$J$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="120">
   <si>
     <t>BACKLOG</t>
   </si>
@@ -637,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -732,14 +734,56 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -884,6 +928,406 @@
           <c:cat>
             <c:strRef>
               <c:f>HFSystem!$R$4:$R$8</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HFSystem!$S$4:$S$8</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-331D-440F-B63C-AA26796B96B0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>HFSystem!$R$4:$R$8</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HFSystem!$T$4:$T$8</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-331D-440F-B63C-AA26796B96B0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="186716719"/>
+        <c:axId val="186686959"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="186716719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="186686959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="186686959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="186716719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>BURNDOWN - PRODUTIVIDADE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'HFSystem (2)'!$W$4:$W$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -906,7 +1350,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>HFSystem!$S$4:$S$8</c:f>
+              <c:f>'HFSystem (2)'!$X$4:$X$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -931,7 +1375,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-331D-440F-B63C-AA26796B96B0}"/>
+              <c16:uniqueId val="{00000000-DEE9-4F01-95A1-4EAA4D9A8260}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -969,7 +1413,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-AF22-4347-9949-BD8405753293}"/>
+                  <c16:uniqueId val="{00000001-DEE9-4F01-95A1-4EAA4D9A8260}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -991,7 +1435,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-AF22-4347-9949-BD8405753293}"/>
+                  <c16:uniqueId val="{00000002-DEE9-4F01-95A1-4EAA4D9A8260}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1013,7 +1457,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-AF22-4347-9949-BD8405753293}"/>
+                  <c16:uniqueId val="{00000003-DEE9-4F01-95A1-4EAA4D9A8260}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1035,7 +1479,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-AF22-4347-9949-BD8405753293}"/>
+                  <c16:uniqueId val="{00000004-DEE9-4F01-95A1-4EAA4D9A8260}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1057,7 +1501,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-AF22-4347-9949-BD8405753293}"/>
+                  <c16:uniqueId val="{00000005-DEE9-4F01-95A1-4EAA4D9A8260}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1120,7 +1564,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>HFSystem!$R$4:$R$8</c:f>
+              <c:f>'HFSystem (2)'!$W$4:$W$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1143,7 +1587,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>HFSystem!$T$4:$T$8</c:f>
+              <c:f>'HFSystem (2)'!$Y$4:$Y$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1168,7 +1612,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-331D-440F-B63C-AA26796B96B0}"/>
+              <c16:uniqueId val="{00000006-DEE9-4F01-95A1-4EAA4D9A8260}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1414,7 +1858,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1973,6 +2973,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>6484</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>8106</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>824753</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>63168</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D1A5E32-5820-4B31-8C14-0F0DCF0B402B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2236,10 +3279,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="B1:U46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2339,7 +3383,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B4" s="11" t="s">
         <v>59</v>
       </c>
@@ -2387,7 +3431,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="2:21" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:21" s="13" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
         <v>60</v>
       </c>
@@ -2436,7 +3480,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B6" s="11" t="s">
         <v>58</v>
       </c>
@@ -2485,7 +3529,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B7" s="11" t="s">
         <v>61</v>
       </c>
@@ -2530,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>67</v>
       </c>
@@ -2574,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B9" s="11" t="s">
         <v>83</v>
       </c>
@@ -2607,7 +3651,7 @@
       <c r="L9" s="17"/>
       <c r="P9" s="18"/>
     </row>
-    <row r="10" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B10" s="11" t="s">
         <v>62</v>
       </c>
@@ -2640,7 +3684,7 @@
       <c r="L10" s="17"/>
       <c r="P10" s="18"/>
     </row>
-    <row r="11" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B11" s="11" t="s">
         <v>63</v>
       </c>
@@ -2673,7 +3717,7 @@
       <c r="L11" s="17"/>
       <c r="P11" s="18"/>
     </row>
-    <row r="12" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B12" s="11" t="s">
         <v>64</v>
       </c>
@@ -2706,7 +3750,7 @@
       <c r="L12" s="17"/>
       <c r="P12" s="18"/>
     </row>
-    <row r="13" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
         <v>65</v>
       </c>
@@ -2739,7 +3783,7 @@
       <c r="L13" s="17"/>
       <c r="P13" s="18"/>
     </row>
-    <row r="14" spans="2:21" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:21" s="13" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B14" s="12" t="s">
         <v>66</v>
       </c>
@@ -2775,7 +3819,7 @@
       <c r="O14" s="9"/>
       <c r="P14" s="18"/>
     </row>
-    <row r="15" spans="2:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:21" ht="18.600000000000001" hidden="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="11" t="s">
         <v>68</v>
       </c>
@@ -2811,7 +3855,7 @@
       <c r="O15" s="22"/>
       <c r="P15" s="23"/>
     </row>
-    <row r="16" spans="2:21" ht="18" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:21" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B16" s="11" t="s">
         <v>69</v>
       </c>
@@ -2843,7 +3887,7 @@
       <c r="K16" s="10"/>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B17" s="11" t="s">
         <v>70</v>
       </c>
@@ -2874,7 +3918,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B18" s="11" t="s">
         <v>71</v>
       </c>
@@ -3370,7 +4414,7 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B34" s="11" t="s">
         <v>29</v>
       </c>
@@ -3401,7 +4445,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B35" s="11" t="s">
         <v>30</v>
       </c>
@@ -3432,11 +4476,11 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B36" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="11" t="s">
         <v>118</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -3463,7 +4507,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B37" s="11" t="s">
         <v>32</v>
       </c>
@@ -3494,7 +4538,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B38" s="11" t="s">
         <v>33</v>
       </c>
@@ -3525,7 +4569,7 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B39" s="11" t="s">
         <v>76</v>
       </c>
@@ -3556,7 +4600,7 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B40" s="11" t="s">
         <v>77</v>
       </c>
@@ -3587,7 +4631,7 @@
       </c>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B41" s="11" t="s">
         <v>78</v>
       </c>
@@ -3618,7 +4662,7 @@
       </c>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B42" s="11" t="s">
         <v>79</v>
       </c>
@@ -3649,7 +4693,7 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
@@ -3680,7 +4724,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B44" s="11" t="s">
         <v>81</v>
       </c>
@@ -3711,7 +4755,7 @@
       </c>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B45" s="11" t="s">
         <v>82</v>
       </c>
@@ -3742,7 +4786,7 @@
       </c>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.45">
       <c r="B46" s="11" t="s">
         <v>34</v>
       </c>
@@ -3774,7 +4818,13 @@
       <c r="K46" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:J46" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="B3:J46" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="SP2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="R2:U2"/>
@@ -3863,6 +4913,1642 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81505AEF-48CF-4C84-B9D1-8C183E32BEB6}">
+  <dimension ref="B1:Z46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AF24" sqref="AF24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="86.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="15" style="9" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" style="9" customWidth="1"/>
+    <col min="16" max="16" width="57" style="9" customWidth="1"/>
+    <col min="17" max="17" width="2.109375" style="9" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.109375" style="9"/>
+    <col min="23" max="23" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.109375" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="W2" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="36"/>
+    </row>
+    <row r="3" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="10"/>
+      <c r="L3" s="17"/>
+      <c r="P3" s="18"/>
+      <c r="W3" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="X3" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y3" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z3" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="6">
+        <f>IF(E4="PP",3,IF(E4="P",5,IF(E4="M",8,IF(E4="G",13,21))))</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="17"/>
+      <c r="P4" s="18"/>
+      <c r="W4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="X4" s="14">
+        <f>X5+X6+X7</f>
+        <v>449</v>
+      </c>
+      <c r="Y4" s="14">
+        <f>SUM(Y5:Y7)</f>
+        <v>449</v>
+      </c>
+      <c r="Z4" s="14">
+        <f>SUM(Z5:Z8)</f>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
+      <c r="B5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" ref="F5:F46" si="0">IF(E5="PP",3,IF(E5="P",5,IF(E5="M",8,IF(E5="G",13,21))))</f>
+        <v>13</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="17"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="18"/>
+      <c r="W5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="14">
+        <f>149</f>
+        <v>149</v>
+      </c>
+      <c r="Y5" s="15">
+        <f>SUM(F4:F18)</f>
+        <v>118</v>
+      </c>
+      <c r="Z5" s="14">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="19"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="20"/>
+      <c r="W6" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="X6" s="14">
+        <f>150</f>
+        <v>150</v>
+      </c>
+      <c r="Y6" s="15">
+        <f>SUM(F19:F33)</f>
+        <v>134</v>
+      </c>
+      <c r="Z6" s="14">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="17"/>
+      <c r="P7" s="18"/>
+      <c r="W7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="X7" s="14">
+        <v>150</v>
+      </c>
+      <c r="Y7" s="15">
+        <f>SUM(F34:F46)</f>
+        <v>197</v>
+      </c>
+      <c r="Z7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" ht="18" x14ac:dyDescent="0.3">
+      <c r="B8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="P8" s="18"/>
+      <c r="W8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="X8" s="14">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="17"/>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="17"/>
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="17"/>
+      <c r="P11" s="18"/>
+    </row>
+    <row r="12" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="17"/>
+      <c r="P12" s="18"/>
+    </row>
+    <row r="13" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B13" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G13" s="4">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="17"/>
+      <c r="P13" s="18"/>
+    </row>
+    <row r="14" spans="2:26" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
+      <c r="B14" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="18"/>
+    </row>
+    <row r="15" spans="2:26" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="23"/>
+    </row>
+    <row r="16" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="B16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="Q16" s="16"/>
+    </row>
+    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B20" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G20" s="4">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G25" s="4">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B26" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B27" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G27" s="4">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B28" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G28" s="4">
+        <v>2</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B29" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K29" s="10"/>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G30" s="4">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B31" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G31" s="4">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B32" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B33" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G33" s="4">
+        <v>3</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B34" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G34" s="4">
+        <v>2</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B35" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G35" s="4">
+        <v>3</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K35" s="10"/>
+    </row>
+    <row r="36" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B36" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G36" s="4">
+        <v>2</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K36" s="10"/>
+    </row>
+    <row r="37" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B37" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G37" s="4">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K37" s="10"/>
+    </row>
+    <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G38" s="4">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K38" s="10"/>
+    </row>
+    <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B39" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G39" s="4">
+        <v>2</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K39" s="10"/>
+    </row>
+    <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B40" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G40" s="4">
+        <v>3</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K40" s="10"/>
+    </row>
+    <row r="41" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B41" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G41" s="4">
+        <v>2</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K41" s="10"/>
+    </row>
+    <row r="42" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B42" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G42" s="4">
+        <v>2</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K42" s="10"/>
+    </row>
+    <row r="43" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B43" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G43" s="4">
+        <v>1</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K43" s="10"/>
+    </row>
+    <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B44" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K44" s="10"/>
+    </row>
+    <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B45" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G45" s="4">
+        <v>1</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="B46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K46" s="10"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B3:J46" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <mergeCells count="3">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="L2:T2"/>
+  </mergeCells>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H46" xr:uid="{79424059-AB6B-4E53-AF77-2D9BC4B5C855}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E46" xr:uid="{761344AA-9997-4D07-9411-4F798FBE6840}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{E635083B-E0A4-4756-976C-204B43713309}">
+            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$3,J4)))</xm:f>
+            <xm:f>'Banco de dados'!$B$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{1F24DF79-5618-4E43-B4EE-AC3EAC612ECF}">
+            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$4,J4)))</xm:f>
+            <xm:f>'Banco de dados'!$B$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF00B050"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{F3DD79D6-9256-414E-A886-F5F17830A2EA}">
+            <xm:f>NOT(ISERROR(SEARCH('Banco de dados'!$B$2,J4)))</xm:f>
+            <xm:f>'Banco de dados'!$B$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J4:J46</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC4079D4-97D3-4036-9C61-25CCB9465A16}">
+          <x14:formula1>
+            <xm:f>'Banco de dados'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4:D46</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49439B0F-C39F-45CD-B22F-F15D911B1852}">
+          <x14:formula1>
+            <xm:f>'Banco de dados'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>J4:J46</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B0F8FD-0295-424D-BFA2-4D3F6325DB71}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Alterações das informações do backlog
</commit_message>
<xml_diff>
--- a/Documentacao/Sprint 2/Backlog/HFSystem_Backlog.xlsx
+++ b/Documentacao/Sprint 2/Backlog/HFSystem_Backlog.xlsx
@@ -5,21 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\SPtech\HFSystem\Documentacao\Sprint 2\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\OneDrive\Pessoal\1 - Documentos\2 - Acessos\Desktop\Projetos\Projetos em grupo\HFSystem\Documentacao\Sprint 2\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED625A1-3058-4C4D-9028-AA950374FD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EE869E-8AC5-4976-9CDC-784C0E5D2F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5184" yWindow="348" windowWidth="17856" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFSystem" sheetId="1" r:id="rId1"/>
-    <sheet name="HFSystem (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="DASHBOARD" sheetId="3" r:id="rId2"/>
     <sheet name="Banco de dados" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DASHBOARD!$B$3:$J$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HFSystem!$B$3:$J$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'HFSystem (2)'!$B$3:$J$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -408,7 +408,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,6 +462,33 @@
       <name val="Arial Nova Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial Nova Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial Nova Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Yu Gothic Medium"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -489,7 +516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -635,11 +662,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0E617C"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0E617C"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0E617C"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0E617C"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF0E617C"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,9 +780,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,12 +789,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -747,6 +796,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -925,11 +1019,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>HFSystem!$R$4:$R$8</c:f>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>HFSystem!$S$4:$S$8</c:f>
@@ -937,6 +1026,21 @@
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>HFSystem!$R$4:$R$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:multiLvlStrRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-331D-440F-B63C-AA26796B96B0}"/>
             </c:ext>
@@ -1015,11 +1119,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>HFSystem!$R$4:$R$8</c:f>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>HFSystem!$T$4:$T$8</c:f>
@@ -1027,6 +1126,21 @@
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>HFSystem!$R$4:$R$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:multiLvlStrRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-331D-440F-B63C-AA26796B96B0}"/>
             </c:ext>
@@ -1256,7 +1370,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1269,7 +1383,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:rPr lang="pt-BR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
               <a:t>BURNDOWN - PRODUTIVIDADE</a:t>
             </a:r>
           </a:p>
@@ -1288,7 +1402,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1313,6 +1427,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Planejado</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1327,7 +1444,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'HFSystem (2)'!$W$4:$W$8</c:f>
+              <c:f>DASHBOARD!$V$4:$V$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1350,7 +1467,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'HFSystem (2)'!$X$4:$X$8</c:f>
+              <c:f>DASHBOARD!$W$4:$W$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1382,6 +1499,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Realizado</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1519,7 +1639,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1564,7 +1684,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'HFSystem (2)'!$W$4:$W$8</c:f>
+              <c:f>DASHBOARD!$V$4:$V$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1587,7 +1707,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'HFSystem (2)'!$Y$4:$Y$8</c:f>
+              <c:f>DASHBOARD!$X$4:$X$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1657,7 +1777,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1716,7 +1836,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1758,7 +1878,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2986,7 +3106,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>824753</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>63168</xdr:rowOff>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3282,8 +3402,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B1:U46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView showGridLines="0" zoomScale="113" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3298,16 +3418,16 @@
     <col min="9" max="9" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.109375" style="9" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="15" style="9" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" style="9" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="9"/>
-    <col min="17" max="17" width="2.109375" style="9" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="9" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="9" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="9" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" style="9" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="0" style="9" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.109375" style="9" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" style="9" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="9" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" style="9" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" style="9" hidden="1" customWidth="1"/>
     <col min="22" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
@@ -3325,19 +3445,19 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="R2" s="28" t="s">
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="R2" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
     </row>
     <row r="3" spans="2:21" ht="18" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
@@ -3957,7 +4077,7 @@
         <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>50</v>
@@ -3976,7 +4096,7 @@
         <v>93</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K19" s="10"/>
     </row>
@@ -3988,7 +4108,7 @@
         <v>107</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>52</v>
@@ -4007,7 +4127,7 @@
         <v>89</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K20" s="10"/>
     </row>
@@ -4019,7 +4139,7 @@
         <v>111</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>53</v>
@@ -4038,7 +4158,7 @@
         <v>92</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K21" s="10"/>
     </row>
@@ -4050,7 +4170,7 @@
         <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>53</v>
@@ -4069,7 +4189,7 @@
         <v>92</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K22" s="10"/>
     </row>
@@ -4081,7 +4201,7 @@
         <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>53</v>
@@ -4100,7 +4220,7 @@
         <v>92</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K23" s="10"/>
     </row>
@@ -4112,7 +4232,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>52</v>
@@ -4131,7 +4251,7 @@
         <v>88</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K24" s="10"/>
     </row>
@@ -4143,7 +4263,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>52</v>
@@ -4162,7 +4282,7 @@
         <v>90</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K25" s="10"/>
     </row>
@@ -4174,7 +4294,7 @@
         <v>40</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>51</v>
@@ -4193,7 +4313,7 @@
         <v>89</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K26" s="10"/>
     </row>
@@ -4205,7 +4325,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>50</v>
@@ -4224,7 +4344,7 @@
         <v>91</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K27" s="10"/>
     </row>
@@ -4236,7 +4356,7 @@
         <v>108</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>52</v>
@@ -4255,7 +4375,7 @@
         <v>93</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K28" s="10"/>
     </row>
@@ -4267,7 +4387,7 @@
         <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>53</v>
@@ -4286,7 +4406,7 @@
         <v>89</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K29" s="10"/>
     </row>
@@ -4298,7 +4418,7 @@
         <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>51</v>
@@ -4317,7 +4437,7 @@
         <v>91</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K30" s="10"/>
     </row>
@@ -4329,7 +4449,7 @@
         <v>43</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>53</v>
@@ -4348,7 +4468,7 @@
         <v>88</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K31" s="10"/>
     </row>
@@ -4360,7 +4480,7 @@
         <v>44</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>53</v>
@@ -4379,7 +4499,7 @@
         <v>93</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K32" s="10"/>
     </row>
@@ -4391,7 +4511,7 @@
         <v>45</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>52</v>
@@ -4410,7 +4530,7 @@
         <v>90</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K33" s="10"/>
     </row>
@@ -4916,22 +5036,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81505AEF-48CF-4C84-B9D1-8C183E32BEB6}">
   <dimension ref="B1:Z46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AF24" sqref="AF24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.44140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="86.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="123.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="79.5546875" style="9" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="119.6640625" style="9" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="9" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="16.77734375" style="9" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" style="9" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" style="9" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="2.109375" style="9" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.44140625" style="9" customWidth="1"/>
     <col min="14" max="14" width="15" style="9" customWidth="1"/>
@@ -4941,48 +5061,48 @@
     <col min="18" max="18" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" style="9" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.109375" style="9"/>
-    <col min="23" max="23" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.6640625" style="9" customWidth="1"/>
+    <col min="22" max="22" width="13" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.6640625" style="9" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="13.33203125" style="9" customWidth="1"/>
     <col min="27" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:26" ht="18" x14ac:dyDescent="0.45">
-      <c r="B2" s="25" t="s">
+    <row r="1" spans="2:25" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:25" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="48"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="W2" s="34" t="s">
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="36"/>
+      <c r="V2" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="36"/>
-    </row>
-    <row r="3" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="42"/>
+    </row>
+    <row r="3" spans="2:25" ht="19.2" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5012,21 +5132,28 @@
       </c>
       <c r="K3" s="10"/>
       <c r="L3" s="17"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
       <c r="P3" s="18"/>
-      <c r="W3" s="24" t="s">
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="18"/>
+      <c r="V3" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="X3" s="24" t="s">
+      <c r="W3" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="Y3" s="24" t="s">
+      <c r="X3" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="Z3" s="24" t="s">
+      <c r="Y3" s="43" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:25" ht="19.2" x14ac:dyDescent="0.45">
       <c r="B4" s="11" t="s">
         <v>59</v>
       </c>
@@ -5057,24 +5184,31 @@
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="17"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
       <c r="P4" s="18"/>
-      <c r="W4" s="14" t="s">
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="18"/>
+      <c r="V4" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="X4" s="14">
-        <f>X5+X6+X7</f>
+      <c r="W4" s="44">
+        <f>W5+W6+W7</f>
         <v>449</v>
       </c>
-      <c r="Y4" s="14">
-        <f>SUM(Y5:Y7)</f>
+      <c r="X4" s="44">
+        <f>SUM(X5:X7)</f>
         <v>449</v>
       </c>
-      <c r="Z4" s="14">
-        <f>SUM(Z5:Z8)</f>
+      <c r="Y4" s="44">
+        <f>SUM(Y5:Y8)</f>
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="2:26" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:25" s="13" customFormat="1" ht="22.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="12" t="s">
         <v>60</v>
       </c>
@@ -5104,26 +5238,30 @@
         <v>103</v>
       </c>
       <c r="L5" s="17"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
       <c r="P5" s="18"/>
-      <c r="W5" s="14" t="s">
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="20"/>
+      <c r="V5" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="X5" s="14">
+      <c r="W5" s="44">
         <f>149</f>
         <v>149</v>
       </c>
-      <c r="Y5" s="15">
+      <c r="X5" s="45">
         <f>SUM(F4:F18)</f>
         <v>118</v>
       </c>
-      <c r="Z5" s="14">
+      <c r="Y5" s="44">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:25" ht="22.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="11" t="s">
         <v>58</v>
       </c>
@@ -5153,26 +5291,30 @@
         <v>103</v>
       </c>
       <c r="L6" s="19"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
       <c r="P6" s="20"/>
-      <c r="W6" s="14" t="s">
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="18"/>
+      <c r="V6" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="X6" s="14">
+      <c r="W6" s="44">
         <f>150</f>
         <v>150</v>
       </c>
-      <c r="Y6" s="15">
+      <c r="X6" s="45">
         <f>SUM(F19:F33)</f>
         <v>134</v>
       </c>
-      <c r="Z6" s="14">
+      <c r="Y6" s="44">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:25" ht="22.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="11" t="s">
         <v>61</v>
       </c>
@@ -5202,22 +5344,29 @@
         <v>103</v>
       </c>
       <c r="L7" s="17"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
       <c r="P7" s="18"/>
-      <c r="W7" s="14" t="s">
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="18"/>
+      <c r="V7" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="X7" s="14">
+      <c r="W7" s="44">
         <v>150</v>
       </c>
-      <c r="Y7" s="15">
+      <c r="X7" s="45">
         <f>SUM(F34:F46)</f>
         <v>197</v>
       </c>
-      <c r="Z7" s="14">
+      <c r="Y7" s="44">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:25" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>67</v>
       </c>
@@ -5247,21 +5396,28 @@
         <v>103</v>
       </c>
       <c r="L8" s="17"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
       <c r="P8" s="18"/>
-      <c r="W8" s="14" t="s">
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="18"/>
+      <c r="V8" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="X8" s="14">
+      <c r="W8" s="44">
         <v>0</v>
       </c>
-      <c r="Y8" s="14">
+      <c r="X8" s="44">
         <v>0</v>
       </c>
-      <c r="Z8" s="14">
+      <c r="Y8" s="44">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:25" ht="18" x14ac:dyDescent="0.45">
       <c r="B9" s="11" t="s">
         <v>83</v>
       </c>
@@ -5292,9 +5448,16 @@
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="17"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
       <c r="P9" s="18"/>
-    </row>
-    <row r="10" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="18"/>
+    </row>
+    <row r="10" spans="2:25" ht="18" x14ac:dyDescent="0.45">
       <c r="B10" s="11" t="s">
         <v>62</v>
       </c>
@@ -5325,9 +5488,16 @@
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="17"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
       <c r="P10" s="18"/>
-    </row>
-    <row r="11" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="18"/>
+    </row>
+    <row r="11" spans="2:25" ht="18" x14ac:dyDescent="0.45">
       <c r="B11" s="11" t="s">
         <v>63</v>
       </c>
@@ -5358,9 +5528,16 @@
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="17"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
       <c r="P11" s="18"/>
-    </row>
-    <row r="12" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="18"/>
+    </row>
+    <row r="12" spans="2:25" ht="18" x14ac:dyDescent="0.45">
       <c r="B12" s="11" t="s">
         <v>64</v>
       </c>
@@ -5391,9 +5568,16 @@
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="17"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
       <c r="P12" s="18"/>
-    </row>
-    <row r="13" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="18"/>
+    </row>
+    <row r="13" spans="2:25" ht="18" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
         <v>65</v>
       </c>
@@ -5424,9 +5608,16 @@
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="17"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
       <c r="P13" s="18"/>
-    </row>
-    <row r="14" spans="2:26" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="18"/>
+    </row>
+    <row r="14" spans="2:25" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.45">
       <c r="B14" s="12" t="s">
         <v>66</v>
       </c>
@@ -5457,12 +5648,16 @@
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="17"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
       <c r="P14" s="18"/>
-    </row>
-    <row r="15" spans="2:26" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="20"/>
+    </row>
+    <row r="15" spans="2:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="11" t="s">
         <v>68</v>
       </c>
@@ -5497,8 +5692,12 @@
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
       <c r="P15" s="23"/>
-    </row>
-    <row r="16" spans="2:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="18"/>
+    </row>
+    <row r="16" spans="2:25" ht="18" x14ac:dyDescent="0.45">
       <c r="B16" s="11" t="s">
         <v>69</v>
       </c>
@@ -5528,9 +5727,17 @@
         <v>103</v>
       </c>
       <c r="K16" s="10"/>
-      <c r="Q16" s="16"/>
-    </row>
-    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L16" s="17"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="18"/>
+    </row>
+    <row r="17" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B17" s="11" t="s">
         <v>70</v>
       </c>
@@ -5560,8 +5767,17 @@
         <v>103</v>
       </c>
       <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L17" s="17"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="18"/>
+    </row>
+    <row r="18" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B18" s="11" t="s">
         <v>71</v>
       </c>
@@ -5591,8 +5807,17 @@
         <v>103</v>
       </c>
       <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L18" s="17"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="18"/>
+    </row>
+    <row r="19" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B19" s="11" t="s">
         <v>18</v>
       </c>
@@ -5600,7 +5825,7 @@
         <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>50</v>
@@ -5619,11 +5844,20 @@
         <v>93</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L19" s="17"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="18"/>
+    </row>
+    <row r="20" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
@@ -5631,7 +5865,7 @@
         <v>107</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>52</v>
@@ -5650,11 +5884,20 @@
         <v>89</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L20" s="17"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="18"/>
+    </row>
+    <row r="21" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
@@ -5662,7 +5905,7 @@
         <v>111</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>53</v>
@@ -5681,11 +5924,20 @@
         <v>92</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K21" s="10"/>
-    </row>
-    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L21" s="17"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="18"/>
+    </row>
+    <row r="22" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
@@ -5693,7 +5945,7 @@
         <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>53</v>
@@ -5712,11 +5964,20 @@
         <v>92</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K22" s="10"/>
-    </row>
-    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L22" s="17"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="18"/>
+    </row>
+    <row r="23" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
@@ -5724,7 +5985,7 @@
         <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>53</v>
@@ -5743,11 +6004,20 @@
         <v>92</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K23" s="10"/>
-    </row>
-    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L23" s="17"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="18"/>
+    </row>
+    <row r="24" spans="2:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B24" s="11" t="s">
         <v>23</v>
       </c>
@@ -5755,7 +6025,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>52</v>
@@ -5774,11 +6044,20 @@
         <v>88</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K24" s="10"/>
-    </row>
-    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+      <c r="L24" s="21"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="23"/>
+    </row>
+    <row r="25" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B25" s="11" t="s">
         <v>24</v>
       </c>
@@ -5786,7 +6065,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>52</v>
@@ -5805,11 +6084,11 @@
         <v>90</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B26" s="11" t="s">
         <v>72</v>
       </c>
@@ -5817,7 +6096,7 @@
         <v>40</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>51</v>
@@ -5836,11 +6115,11 @@
         <v>89</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B27" s="11" t="s">
         <v>25</v>
       </c>
@@ -5848,7 +6127,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>50</v>
@@ -5867,11 +6146,11 @@
         <v>91</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B28" s="11" t="s">
         <v>73</v>
       </c>
@@ -5879,7 +6158,7 @@
         <v>108</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>52</v>
@@ -5898,11 +6177,11 @@
         <v>93</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B29" s="11" t="s">
         <v>74</v>
       </c>
@@ -5910,7 +6189,7 @@
         <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>53</v>
@@ -5929,11 +6208,11 @@
         <v>89</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B30" s="11" t="s">
         <v>26</v>
       </c>
@@ -5941,7 +6220,7 @@
         <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>51</v>
@@ -5960,11 +6239,11 @@
         <v>91</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B31" s="11" t="s">
         <v>27</v>
       </c>
@@ -5972,7 +6251,7 @@
         <v>43</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>53</v>
@@ -5991,11 +6270,11 @@
         <v>88</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:20" ht="18" x14ac:dyDescent="0.45">
       <c r="B32" s="11" t="s">
         <v>75</v>
       </c>
@@ -6003,7 +6282,7 @@
         <v>44</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>53</v>
@@ -6022,7 +6301,7 @@
         <v>93</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K32" s="10"/>
     </row>
@@ -6034,7 +6313,7 @@
         <v>45</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>52</v>
@@ -6464,10 +6743,10 @@
   <autoFilter ref="B3:J46" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="W2:Z2"/>
     <mergeCell ref="L2:T2"/>
+    <mergeCell ref="V2:Y2"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H46" xr:uid="{79424059-AB6B-4E53-AF77-2D9BC4B5C855}">
       <formula1>#REF!</formula1>
     </dataValidation>
@@ -6529,7 +6808,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC4079D4-97D3-4036-9C61-25CCB9465A16}">
           <x14:formula1>
             <xm:f>'Banco de dados'!$A$2:$A$4</xm:f>

</xml_diff>